<commit_message>
Upload last changes 05.07.2022
</commit_message>
<xml_diff>
--- a/assets/files/maestros/Campaña.xlsx
+++ b/assets/files/maestros/Campaña.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\maestros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA82012-E982-46FE-8C57-16DD7FD7EFBA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B643828-5D25-400C-A876-C3A800080D57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,13 +45,17 @@
     <t>mensaje_video</t>
   </si>
   <si>
-    <t>HOLA! Celebra Fiestas Patrias con  XION\u{1F973} \u{1F1F5}\u{1F1EA} &lt;br&gt;\
-Solo por esta semana nuestra Silla Gamer Raven disponible en todos los colores. \u{1F440} &lt;br&gt;\
-VIVE ESTA EXPERIENCIA AL MÁXIMO ‼️ &lt;br&gt;\
-NO ESPERES MÁS Y OBTÉN LA TUYA.</t>
+    <t>C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\campaña\video_decokasa.mp4</t>
   </si>
   <si>
-    <t>C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\campaña\i3_campaña2.jpg</t>
+    <t>\u{1F4A5}Llegaron los descuentos más esperados del año \u{1F4A5} #CYBERWOW \n\
+¡PISOS AUTOADHESIVOS DE PVC!  \n\
+Válido del 04/07/22 al 08/07/22 en nuestra tienda y WhatsApp. \n\
+Aprovecha el Cyber WOW y Remodela tu Hogar. \n\
+\u{1F4F2} WhatsApp: 947 154 969 \n\
+Whatsapp: https://bit.ly/DECO_MAYORISTAS_PISOS \n\
+Tienda física en: Av. Benavides 1980 – Miraflores \n\
+Envíos a todo el Perú \u{1F6F5}</t>
   </si>
 </sst>
 </file>
@@ -121,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -144,6 +148,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -429,16 +436,16 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" customWidth="1"/>
     <col min="2" max="2" width="94.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.7109375" customWidth="1"/>
+    <col min="5" max="5" width="91.42578125" customWidth="1"/>
     <col min="6" max="6" width="98.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -463,15 +470,15 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix error scraping, update
</commit_message>
<xml_diff>
--- a/assets/files/maestros/Campaña.xlsx
+++ b/assets/files/maestros/Campaña.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\maestros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B643828-5D25-400C-A876-C3A800080D57}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19726DFD-C303-49BA-B773-B065975AF8A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,24 +50,17 @@
     <t>mensaje_video</t>
   </si>
   <si>
-    <t>C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\campaña\video_decokasa.mp4</t>
+    <t>C:\Users\Personal\Documents\PythonProjects\AppScraping\assets\files\campaña\diciembre_flavia.jpg</t>
   </si>
   <si>
-    <t>\u{1F4A5}Llegaron los descuentos más esperados del año \u{1F4A5} #CYBERWOW \n\
-¡PISOS AUTOADHESIVOS DE PVC!  \n\
-Válido del 04/07/22 al 08/07/22 en nuestra tienda y WhatsApp. \n\
-Aprovecha el Cyber WOW y Remodela tu Hogar. \n\
-\u{1F4F2} WhatsApp: 947 154 969 \n\
-Whatsapp: https://bit.ly/DECO_MAYORISTAS_PISOS \n\
-Tienda física en: Av. Benavides 1980 – Miraflores \n\
-Envíos a todo el Perú \u{1F6F5}</t>
+    <t>\u{1F6A8}SUPER DESCUENTOS POR FIN DE AÑO\u{1F6A8} pusimos todos nuestros productos en oferta al por mayor.\u{1F631} Aprovecha para abastecer tu negocio con estas súper promociones. Valido solo hasta el 31 de diciembre.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +76,21 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -125,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -141,17 +154,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,14 +451,14 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.85546875" customWidth="1"/>
     <col min="2" max="2" width="94.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.7109375" customWidth="1"/>
     <col min="5" max="5" width="91.42578125" customWidth="1"/>
     <col min="6" max="6" width="98.5703125" bestFit="1" customWidth="1"/>
@@ -469,36 +484,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="114" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="7" t="s">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="7"/>
+      <c r="D2" s="12"/>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="10"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -526,7 +538,7 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>